<commit_message>
ok we done now
</commit_message>
<xml_diff>
--- a/Stats/R/HW 2/Births.xlsx
+++ b/Stats/R/HW 2/Births.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/striola/Dropbox/Triola Stats/Books/ES 13e/13e Working Docs/App B Data Sets/Excel/ES13 Data Sets Excel FINAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dal866445\Documents\GitHub\yahriels\Stats\R\HW 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381AC193-D161-41F3-ADA7-01CA96FCC38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="480" windowWidth="14360" windowHeight="17420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="04 - Births" sheetId="1" r:id="rId1"/>
@@ -80,9 +81,6 @@
     <t>FACILITY</t>
   </si>
   <si>
-    <t>GENDER (1=M)</t>
-  </si>
-  <si>
     <t>LENGTH OF STAY</t>
   </si>
   <si>
@@ -97,11 +95,14 @@
   <si>
     <t>TOTAL CHARGES</t>
   </si>
+  <si>
+    <t>GENDER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -165,6 +166,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -432,27 +436,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="15.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -460,25 +464,25 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,7 +508,7 @@
         <v>13985.7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,7 +534,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -556,7 +560,7 @@
         <v>359091</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -582,7 +586,7 @@
         <v>8536.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +612,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +638,7 @@
         <v>6406</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,7 +664,7 @@
         <v>4778</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -686,7 +690,7 @@
         <v>3528</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -712,7 +716,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +742,7 @@
         <v>6073.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,7 +768,7 @@
         <v>149241</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -790,7 +794,7 @@
         <v>5122.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -816,7 +820,7 @@
         <v>6986.9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -842,7 +846,7 @@
         <v>4615.1000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -868,7 +872,7 @@
         <v>5488</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +898,7 @@
         <v>3239</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -920,7 +924,7 @@
         <v>4778</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -946,7 +950,7 @@
         <v>7113.05</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -972,7 +976,7 @@
         <v>7367</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>5082.38</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>3733.42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>31766.1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>27561.8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>10144.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>52868.4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>97901</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1184,7 @@
         <v>5488</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>4260.3999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1236,7 @@
         <v>15484.5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>5130</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>106492</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1314,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>6907.1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +1366,7 @@
         <v>8313.8799999999992</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>255788</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>4737.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Stats HW Recovered yay!
</commit_message>
<xml_diff>
--- a/Stats/R/HW 2/Births.xlsx
+++ b/Stats/R/HW 2/Births.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dal866445\Documents\GitHub\yahriels\Stats\R\HW 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahri\yahriels\Stats\R\HW 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381AC193-D161-41F3-ADA7-01CA96FCC38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C871F-EF00-4C9B-B24F-74F86B38B58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="04 - Births" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
     <t>TOTAL CHARGES</t>
   </si>
   <si>
-    <t>GENDER</t>
+    <t>GENDER (1=M)</t>
   </si>
 </sst>
 </file>
@@ -443,20 +443,20 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.08203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="7" max="7" width="15.58203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -482,7 +482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,7 +508,7 @@
         <v>13985.7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,7 +560,7 @@
         <v>359091</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,7 +586,7 @@
         <v>8536.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -638,7 +638,7 @@
         <v>6406</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -664,7 +664,7 @@
         <v>4778</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>3528</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -716,7 +716,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -742,7 +742,7 @@
         <v>6073.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -768,7 +768,7 @@
         <v>149241</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -794,7 +794,7 @@
         <v>5122.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -820,7 +820,7 @@
         <v>6986.9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,7 +846,7 @@
         <v>4615.1000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -872,7 +872,7 @@
         <v>5488</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -898,7 +898,7 @@
         <v>3239</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>4778</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -950,7 +950,7 @@
         <v>7113.05</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -976,7 +976,7 @@
         <v>7367</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>5082.38</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>3733.42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>31766.1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>27561.8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>10144.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>52868.4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>97901</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>5488</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>4260.3999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>15484.5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>5130</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>106492</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>6907.1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>8313.8799999999992</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>255788</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>4737.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>114858</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>471062</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>5689.53</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>6227.88</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>3445.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>52019.5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>5989.25</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>0</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>3673</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>6629.13</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>0</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>5365.25</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>3665</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>52722.3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>3491</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>120613</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>2142.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>28295.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>0</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>10140</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>0</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>4066.5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>2743</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>86406.399999999994</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>7596.5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>8209.7999999999993</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>25804.6</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>0</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>3491</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>271863</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>6196.3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>3673</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>247477</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>0</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>3722</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>4923.75</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>3494.5</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>4729</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>3380</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>0</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>3928.5</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>3722</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>0</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>4256.8999999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>0</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>3928.5</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>4720.9399999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>0</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>0</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>0</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>3239.35</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>0</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>3854.5</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>79378</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>0</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>53312.800000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>0</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>0</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>3632.5</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>0</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>21568.7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>0</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>4512.5</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>0</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>5163</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>0</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>21975.4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>0</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>133483</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>12</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>4694.95</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>12</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>2344.38</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>12</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>133584</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>12</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>2220.6799999999998</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>12</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>12</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>15509.1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>12</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>107021</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>12</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>5502.81</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>12</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>7528.28</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>12</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>1561.27</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>12</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>2343.38</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>12</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>17374.5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>12</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>2219.6799999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>12</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>1593.38</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>12</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>2227.2600000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>12</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>5802.48</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>12</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>2219.6799999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>12</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>2219.6799999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>12</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>12</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>1588.42</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>12</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>1433.67</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>12</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>1527.26</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>12</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>1569.22</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>12</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>1546.83</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>12</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>12</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>3625.95</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>12</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>1520.68</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>12</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>3102.85</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>12</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>12</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>12</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>2200.4499999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>12</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>2328.36</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>12</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>12</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>1814.09</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>12</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>12</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>4726.49</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>2643.7</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>12</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>4280.3599999999997</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>12</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>2219.6799999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>12</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>7092.24</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>12</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>14456.9</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>12</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>14607.1</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>12</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>102607</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>12</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>2661.25</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>12</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>12</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>800.45</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>12</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>12</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>5272.96</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>12</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>10088.299999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>12</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>12</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>12</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>1534.84</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>12</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>5460.54</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
         <v>12</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>1561.27</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>12</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>2435.09</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
         <v>12</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>12</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>1520.68</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>12</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>12</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>1534.84</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>12</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>12</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>12</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>1527.26</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
         <v>12</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>1527.26</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>12</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>2219.6799999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>12</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>45966.1</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>12</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>1625.83</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
         <v>12</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>12</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>121349</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
         <v>12</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>1569.22</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
         <v>12</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>3445.32</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
         <v>12</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>9976.24</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>12</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>2220.6799999999998</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
         <v>12</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>4801.1000000000004</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
         <v>12</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
         <v>12</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>2710.79</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>12</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>3474.43</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
         <v>12</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>3819.27</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>12</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>2220.6799999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
         <v>12</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>1500.45</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
         <v>12</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>4714.33</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
         <v>12</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>20950</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
         <v>12</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
         <v>12</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>1520.68</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>12</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>197912</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
         <v>12</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
         <v>12</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>2200.4499999999998</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
         <v>12</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>16230.5</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>12</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>1500.45</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
         <v>12</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>1520.68</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>12</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>8583.1299999999992</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
         <v>12</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" s="2" t="s">
         <v>12</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>1687.06</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="2" t="s">
         <v>12</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>1846.08</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>1621.13</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
         <v>12</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>2234.84</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
         <v>12</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>1627.84</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
         <v>12</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>12</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>1519.68</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
         <v>13</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>2011.5</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>13</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>1333.5</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>13</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>1311.5</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>13</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>1898.5</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>13</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>1253.5</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>13</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>3729</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>13</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>1677.5</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>13</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>13</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>13</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>13</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>13</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>13</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>13</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>13</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>13</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>13</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>13</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>13</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" s="2" t="s">
         <v>13</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>619.5</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
         <v>13</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" s="2" t="s">
         <v>13</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>1353.5</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
         <v>13</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
         <v>13</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>13</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
         <v>13</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
         <v>13</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>13</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>13</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>945.5</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>13</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" s="2" t="s">
         <v>13</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>1150.5</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" s="2" t="s">
         <v>13</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>1468.5</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
         <v>13</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
         <v>13</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
         <v>13</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A237" s="2" t="s">
         <v>13</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>1810.5</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A238" s="2" t="s">
         <v>13</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>13</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A240" s="2" t="s">
         <v>13</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>1173.5</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A241" s="2" t="s">
         <v>13</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A242" s="2" t="s">
         <v>13</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
         <v>13</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>1781.5</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A244" s="2" t="s">
         <v>13</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>1229.5</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A245" s="2" t="s">
         <v>13</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A246" s="2" t="s">
         <v>13</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>2415</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A247" s="2" t="s">
         <v>13</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>1129.5</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
         <v>13</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A249" s="2" t="s">
         <v>13</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>1251.5</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
         <v>13</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>1251.5</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
         <v>13</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>1680.5</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
         <v>13</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>1239.5</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A253" s="2" t="s">
         <v>13</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>13</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>1150.5</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A255" s="2" t="s">
         <v>13</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>1661.5</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A256" s="2" t="s">
         <v>13</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A257" s="2" t="s">
         <v>13</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>1273.5</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
         <v>13</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>1607.5</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A259" s="2" t="s">
         <v>13</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A260" s="2" t="s">
         <v>13</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>1145.5</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A261" s="2" t="s">
         <v>13</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>1650.5</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A262" s="2" t="s">
         <v>13</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>1639.5</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A263" s="2" t="s">
         <v>13</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>1650.5</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A264" s="2" t="s">
         <v>13</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
         <v>13</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A266" s="2" t="s">
         <v>13</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>1301.5</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
         <v>13</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>1258.5</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
         <v>13</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>663.5</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
         <v>13</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>1482.5</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
         <v>13</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
         <v>13</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>1150.5</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
         <v>13</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A273" s="2" t="s">
         <v>13</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>1766.5</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
         <v>13</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
         <v>13</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>1367.5</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
         <v>13</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
         <v>13</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
         <v>13</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A279" s="2" t="s">
         <v>13</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>1420.5</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A280" s="2" t="s">
         <v>13</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>1150.5</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A281" s="2" t="s">
         <v>13</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
         <v>13</v>
       </c>
@@ -7788,7 +7788,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A283" s="2" t="s">
         <v>13</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>3553</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
         <v>13</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A285" s="2" t="s">
         <v>13</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>1831.5</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
         <v>13</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A287" s="2" t="s">
         <v>13</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>1228.5</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
         <v>13</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>2523</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A289" s="2" t="s">
         <v>13</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>1667.5</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
         <v>13</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A291" s="2" t="s">
         <v>13</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>1224.5</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
         <v>13</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>1229.5</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A293" s="2" t="s">
         <v>13</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
         <v>13</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A295" s="2" t="s">
         <v>13</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>1560.5</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A296" s="2" t="s">
         <v>13</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A297" s="2" t="s">
         <v>13</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A298" s="2" t="s">
         <v>13</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>1145.5</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A299" s="2" t="s">
         <v>13</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>1700.5</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A300" s="2" t="s">
         <v>13</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>1670.5</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A301" s="2" t="s">
         <v>13</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>1251.5</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
         <v>15</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A303" s="2" t="s">
         <v>15</v>
       </c>
@@ -8334,7 +8334,7 @@
         <v>2140.39</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A304" s="2" t="s">
         <v>15</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>3221</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A305" s="2" t="s">
         <v>15</v>
       </c>
@@ -8386,7 +8386,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
         <v>15</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A307" s="2" t="s">
         <v>15</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A308" s="2" t="s">
         <v>15</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>2702</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A309" s="2" t="s">
         <v>15</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>3834</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A310" s="2" t="s">
         <v>15</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>3426.6</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A311" s="2" t="s">
         <v>15</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A312" s="2" t="s">
         <v>15</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A313" s="2" t="s">
         <v>15</v>
       </c>
@@ -8594,7 +8594,7 @@
         <v>2497.06</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A314" s="2" t="s">
         <v>15</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A315" s="2" t="s">
         <v>15</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>58461</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A316" s="2" t="s">
         <v>15</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>1497.94</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A317" s="2" t="s">
         <v>15</v>
       </c>
@@ -8698,7 +8698,7 @@
         <v>5742.51</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A318" s="2" t="s">
         <v>15</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>7609.86</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A319" s="2" t="s">
         <v>15</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A320" s="2" t="s">
         <v>15</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>3587</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A321" s="2" t="s">
         <v>15</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
         <v>15</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>11015.1</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A323" s="2" t="s">
         <v>15</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>54164.6</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A324" s="2" t="s">
         <v>15</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>232782</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A325" s="2" t="s">
         <v>15</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A326" s="2" t="s">
         <v>15</v>
       </c>
@@ -8932,7 +8932,7 @@
         <v>2334</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
         <v>15</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>2481.1</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
         <v>15</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>6752</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A329" s="2" t="s">
         <v>15</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
         <v>15</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>17648.2</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A331" s="2" t="s">
         <v>15</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A332" s="2" t="s">
         <v>15</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>3017</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A333" s="2" t="s">
         <v>15</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>12923.1</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A334" s="2" t="s">
         <v>15</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>3844</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A335" s="2" t="s">
         <v>15</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>3877</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
         <v>15</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>2441</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A337" s="2" t="s">
         <v>15</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>2032.5</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A338" s="2" t="s">
         <v>15</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>1934.9</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A339" s="2" t="s">
         <v>15</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>6426.35</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A340" s="2" t="s">
         <v>15</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>2968</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A341" s="2" t="s">
         <v>15</v>
       </c>
@@ -9322,7 +9322,7 @@
         <v>290837</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A342" s="2" t="s">
         <v>15</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A343" s="2" t="s">
         <v>15</v>
       </c>
@@ -9374,7 +9374,7 @@
         <v>5415.59</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
         <v>15</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A345" s="2" t="s">
         <v>15</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
         <v>15</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>36546.6</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A347" s="2" t="s">
         <v>15</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
         <v>15</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>57269.2</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A349" s="2" t="s">
         <v>15</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
         <v>15</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>35528</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A351" s="2" t="s">
         <v>15</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>83735.399999999994</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A352" s="2" t="s">
         <v>15</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A353" s="2" t="s">
         <v>15</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>16512.3</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A354" s="2" t="s">
         <v>15</v>
       </c>
@@ -9660,7 +9660,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A355" s="2" t="s">
         <v>15</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A356" s="2" t="s">
         <v>15</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A357" s="2" t="s">
         <v>15</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
         <v>15</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A359" s="2" t="s">
         <v>15</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A360" s="2" t="s">
         <v>15</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A361" s="2" t="s">
         <v>15</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>3993</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A362" s="2" t="s">
         <v>15</v>
       </c>
@@ -9868,7 +9868,7 @@
         <v>183271</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A363" s="2" t="s">
         <v>15</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A364" s="2" t="s">
         <v>15</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A365" s="2" t="s">
         <v>15</v>
       </c>
@@ -9946,7 +9946,7 @@
         <v>70165.100000000006</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
         <v>15</v>
       </c>
@@ -9972,7 +9972,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A367" s="2" t="s">
         <v>15</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A368" s="2" t="s">
         <v>15</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A369" s="2" t="s">
         <v>15</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>1396.6</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A370" s="2" t="s">
         <v>15</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>3442.4</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A371" s="2" t="s">
         <v>15</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A372" s="2" t="s">
         <v>15</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>36006.699999999997</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A373" s="2" t="s">
         <v>15</v>
       </c>
@@ -10154,7 +10154,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A374" s="2" t="s">
         <v>15</v>
       </c>
@@ -10180,7 +10180,7 @@
         <v>16464.3</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A375" s="2" t="s">
         <v>15</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>17464.900000000001</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A376" s="2" t="s">
         <v>15</v>
       </c>
@@ -10232,7 +10232,7 @@
         <v>5923.59</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A377" s="2" t="s">
         <v>15</v>
       </c>
@@ -10258,7 +10258,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A378" s="2" t="s">
         <v>15</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>5036</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A379" s="2" t="s">
         <v>15</v>
       </c>
@@ -10310,7 +10310,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
         <v>15</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A381" s="2" t="s">
         <v>15</v>
       </c>
@@ -10362,7 +10362,7 @@
         <v>42955.4</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A382" s="2" t="s">
         <v>15</v>
       </c>
@@ -10388,7 +10388,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A383" s="2" t="s">
         <v>15</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A384" s="2" t="s">
         <v>15</v>
       </c>
@@ -10440,7 +10440,7 @@
         <v>68902.8</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A385" s="2" t="s">
         <v>15</v>
       </c>
@@ -10466,7 +10466,7 @@
         <v>1599.9</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A386" s="2" t="s">
         <v>15</v>
       </c>
@@ -10492,7 +10492,7 @@
         <v>155857</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A387" s="2" t="s">
         <v>15</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>2871.82</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A388" s="2" t="s">
         <v>15</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>9032.39</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
         <v>15</v>
       </c>
@@ -10570,7 +10570,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A390" s="2" t="s">
         <v>15</v>
       </c>
@@ -10596,7 +10596,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A391" s="2" t="s">
         <v>15</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A392" s="2" t="s">
         <v>15</v>
       </c>
@@ -10648,7 +10648,7 @@
         <v>48999.4</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A393" s="2" t="s">
         <v>15</v>
       </c>
@@ -10674,7 +10674,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A394" s="2" t="s">
         <v>15</v>
       </c>
@@ -10700,7 +10700,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
         <v>15</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A396" s="2" t="s">
         <v>15</v>
       </c>
@@ -10752,7 +10752,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A397" s="2" t="s">
         <v>15</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
         <v>15</v>
       </c>
@@ -10804,7 +10804,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A399" s="2" t="s">
         <v>15</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A400" s="2" t="s">
         <v>15</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A401" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>